<commit_message>
Diala Add the random.question file
</commit_message>
<xml_diff>
--- a/FlashcardsDAS.xlsx
+++ b/FlashcardsDAS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b9ba356910c535f6/Documents/FHNW/1 Sem 25/Programming/Flash Cards Program/FlashcardDAS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="107" documentId="13_ncr:1_{E260ED6B-C25D-4B16-9D42-2CEB99C38549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5B9F7F4-5D7F-43D6-80A3-A8CAEA74F615}"/>
+  <xr:revisionPtr revIDLastSave="109" documentId="13_ncr:1_{E260ED6B-C25D-4B16-9D42-2CEB99C38549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B1B3F1AA-5CCE-43F3-B1D5-7784E5A88447}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{525EB4BB-E122-46F4-9AC9-49673EF9C31F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{525EB4BB-E122-46F4-9AC9-49673EF9C31F}"/>
   </bookViews>
   <sheets>
     <sheet name="Biology" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
   <si>
     <t>Questions</t>
   </si>
@@ -80,9 +80,6 @@
   </si>
   <si>
     <t>How many chromosomes do humans have?</t>
-  </si>
-  <si>
-    <t>46 (23 pairs)</t>
   </si>
   <si>
     <t>Question</t>
@@ -223,6 +220,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -524,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BBAC9DD-3A3F-4E12-89E9-9D672011EF22}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView zoomScale="76" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" zoomScale="76" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -594,8 +595,8 @@
       <c r="A8" t="s">
         <v>13</v>
       </c>
-      <c r="B8" t="s">
-        <v>14</v>
+      <c r="B8" s="2">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -619,7 +620,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -627,58 +628,58 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
         <v>16</v>
-      </c>
-      <c r="B2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
         <v>18</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
         <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
         <v>22</v>
-      </c>
-      <c r="B5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
         <v>24</v>
-      </c>
-      <c r="B6" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
         <v>26</v>
-      </c>
-      <c r="B7" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
         <v>28</v>
-      </c>
-      <c r="B8" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -690,7 +691,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{638F5298-BB5C-4A89-919E-BB5E81AFA999}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
@@ -710,31 +711,31 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
         <v>30</v>
-      </c>
-      <c r="B2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
         <v>32</v>
-      </c>
-      <c r="B3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" t="s">
         <v>34</v>
-      </c>
-      <c r="B4" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" s="2">
         <v>1492</v>
@@ -742,7 +743,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" s="2">
         <v>1789</v>
@@ -750,15 +751,15 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
         <v>38</v>
-      </c>
-      <c r="B7" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8" s="2">
         <v>1971</v>

</xml_diff>

<commit_message>
Diala Change excel file
</commit_message>
<xml_diff>
--- a/FlashcardsDAS.xlsx
+++ b/FlashcardsDAS.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b9ba356910c535f6/Documents/FHNW/1 Sem 25/Programming/Flash Cards Program/FlashcardDAS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b9ba356910c535f6/Documents/FHNW/1 Sem 25/Programming/Flash Cards Program/FlashcardDAS/FlashcardDAS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="109" documentId="13_ncr:1_{E260ED6B-C25D-4B16-9D42-2CEB99C38549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B1B3F1AA-5CCE-43F3-B1D5-7784E5A88447}"/>
+  <xr:revisionPtr revIDLastSave="111" documentId="13_ncr:1_{E260ED6B-C25D-4B16-9D42-2CEB99C38549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DBF4E836-E649-41BF-8B76-B5B04F2ABBC0}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{525EB4BB-E122-46F4-9AC9-49673EF9C31F}"/>
   </bookViews>
@@ -49,18 +49,12 @@
     <t>What is the largest organ in the human body?</t>
   </si>
   <si>
-    <t>The skin</t>
-  </si>
-  <si>
     <t>How many bones does an adult human body have?</t>
   </si>
   <si>
     <t>Which animal has three hearts?</t>
   </si>
   <si>
-    <t>The octopus</t>
-  </si>
-  <si>
     <t>What pigment makes plants green?</t>
   </si>
   <si>
@@ -158,6 +152,12 @@
   </si>
   <si>
     <t>In what year did women in Switzerland gain the right to vote in federal elections?</t>
+  </si>
+  <si>
+    <t>octopus</t>
+  </si>
+  <si>
+    <t>skin</t>
   </si>
 </sst>
 </file>
@@ -526,7 +526,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="76" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -548,12 +548,12 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2">
         <v>206</v>
@@ -561,39 +561,39 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B8" s="2">
         <v>46</v>
@@ -620,7 +620,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -628,58 +628,58 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -711,31 +711,31 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B5" s="2">
         <v>1492</v>
@@ -743,7 +743,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B6" s="2">
         <v>1789</v>
@@ -751,15 +751,15 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B8" s="2">
         <v>1971</v>

</xml_diff>

<commit_message>
Last version 7-12-2025 ready
</commit_message>
<xml_diff>
--- a/FlashcardsDAS.xlsx
+++ b/FlashcardsDAS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b9ba356910c535f6/Documents/FHNW/1 Sem 25/Programming/Flash Cards Program/FlashcardDAS/FlashcardDAS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="116" documentId="13_ncr:1_{E260ED6B-C25D-4B16-9D42-2CEB99C38549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9FBAA2D1-38DD-414A-B64E-D213A035FC9F}"/>
+  <xr:revisionPtr revIDLastSave="124" documentId="13_ncr:1_{E260ED6B-C25D-4B16-9D42-2CEB99C38549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9F15B45F-B27B-4898-BA69-20B162B92B81}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{525EB4BB-E122-46F4-9AC9-49673EF9C31F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{525EB4BB-E122-46F4-9AC9-49673EF9C31F}"/>
   </bookViews>
   <sheets>
     <sheet name="Biology" sheetId="1" r:id="rId1"/>
@@ -79,24 +79,15 @@
     <t>What is the longest river in the world?</t>
   </si>
   <si>
-    <t>The Nile River</t>
-  </si>
-  <si>
     <t>Which continent has the most countries?</t>
   </si>
   <si>
     <t>Which city is located on two continents?</t>
   </si>
   <si>
-    <t>Istanbul, Turkey (Europe &amp; Asia)</t>
-  </si>
-  <si>
     <t>Which ocean is the largest?</t>
   </si>
   <si>
-    <t>The Pacific Ocean</t>
-  </si>
-  <si>
     <t>Which country has no rivers at all?</t>
   </si>
   <si>
@@ -118,15 +109,9 @@
     <t>What disease killed millions in Europe during the 14th century?</t>
   </si>
   <si>
-    <t>The Black Death (bubonic plague)</t>
-  </si>
-  <si>
     <t>Which wall fell in 1989, marking the beginning of the end of the Cold War?</t>
   </si>
   <si>
-    <t>The Berlin Wall</t>
-  </si>
-  <si>
     <t>Who was the leader of the Soviet Union during World War II?</t>
   </si>
   <si>
@@ -155,6 +140,21 @@
   </si>
   <si>
     <t>Africa</t>
+  </si>
+  <si>
+    <t>Berlin Wall</t>
+  </si>
+  <si>
+    <t>The Black Death</t>
+  </si>
+  <si>
+    <t>Nile</t>
+  </si>
+  <si>
+    <t>Istanbul</t>
+  </si>
+  <si>
+    <t>Pacific</t>
   </si>
 </sst>
 </file>
@@ -515,8 +515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BBAC9DD-3A3F-4E12-89E9-9D672011EF22}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView zoomScale="76" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScale="76" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -538,7 +538,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -554,7 +554,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -621,55 +621,55 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -681,8 +681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{638F5298-BB5C-4A89-919E-BB5E81AFA999}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -702,31 +702,31 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B5" s="1">
         <v>1492</v>
@@ -734,7 +734,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1">
         <v>1789</v>
@@ -742,15 +742,15 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B8" s="1">
         <v>1971</v>

</xml_diff>